<commit_message>
Added Gate Truth Tables to the PDF.
</commit_message>
<xml_diff>
--- a/PDF/Resources/Ternary Logic.xlsx
+++ b/PDF/Resources/Ternary Logic.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="816" windowWidth="19200" windowHeight="7404" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1224" windowWidth="19200" windowHeight="7404" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="90">
   <si>
     <t>FUT</t>
   </si>
@@ -334,15 +334,6 @@
     <t>T&gt;+ = F</t>
   </si>
   <si>
-    <t>N-NOT</t>
-  </si>
-  <si>
-    <t>^</t>
-  </si>
-  <si>
-    <t>F-NOT</t>
-  </si>
-  <si>
     <t>AND</t>
   </si>
   <si>
@@ -352,7 +343,34 @@
     <t>OR</t>
   </si>
   <si>
-    <t>v</t>
+    <t>NNOT</t>
+  </si>
+  <si>
+    <t>FNOT</t>
+  </si>
+  <si>
+    <t>TNOT</t>
+  </si>
+  <si>
+    <t>ISF</t>
+  </si>
+  <si>
+    <t>ISN</t>
+  </si>
+  <si>
+    <t>IST</t>
+  </si>
+  <si>
+    <t>SHIFT_P</t>
+  </si>
+  <si>
+    <t>SHIFT_M</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>SUM_C</t>
   </si>
 </sst>
 </file>
@@ -419,12 +437,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6E0B4"/>
+        <fgColor rgb="FF66FF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -773,57 +791,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -846,85 +818,103 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -942,6 +932,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -954,6 +968,42 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -963,36 +1013,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1000,56 +1020,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1059,9 +1043,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
-      <color rgb="FF66CCFF"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FFFF7C80"/>
+      <color rgb="FF66CCFF"/>
+      <color rgb="FF66FF66"/>
       <color rgb="FFC6E0B4"/>
     </mruColors>
   </colors>
@@ -1389,24 +1374,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="51"/>
-      <c r="G2" s="49" t="s">
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57"/>
+      <c r="G2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="51"/>
-      <c r="L2" s="49" t="s">
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="57"/>
+      <c r="L2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="51"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="57"/>
       <c r="Q2" s="21"/>
       <c r="R2" s="21"/>
       <c r="S2" s="21"/>
@@ -1415,18 +1400,18 @@
       <c r="W2" s="21"/>
       <c r="X2" s="21"/>
       <c r="Y2" s="21"/>
-      <c r="AB2" s="49" t="s">
+      <c r="AB2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="51"/>
-      <c r="AE2" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF2" s="51"/>
-      <c r="AH2" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI2" s="51"/>
+      <c r="AC2" s="57"/>
+      <c r="AE2" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="57"/>
+      <c r="AH2" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI2" s="57"/>
     </row>
     <row r="3" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B3" s="18"/>
@@ -1661,36 +1646,36 @@
       <c r="Y6" s="8"/>
     </row>
     <row r="8" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="51"/>
-      <c r="G8" s="49" t="s">
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
+      <c r="G8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
-      <c r="L8" s="49" t="s">
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="57"/>
+      <c r="L8" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="51"/>
-      <c r="AB8" s="49" t="s">
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="57"/>
+      <c r="AB8" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="AC8" s="51"/>
-      <c r="AE8" s="49" t="s">
+      <c r="AC8" s="57"/>
+      <c r="AE8" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="AF8" s="51"/>
-      <c r="AH8" s="49" t="s">
+      <c r="AF8" s="57"/>
+      <c r="AH8" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="AI8" s="51"/>
+      <c r="AI8" s="57"/>
     </row>
     <row r="9" spans="2:35" x14ac:dyDescent="0.3">
       <c r="B9" s="18"/>
@@ -1893,24 +1878,24 @@
       </c>
     </row>
     <row r="14" spans="2:35" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="51"/>
-      <c r="G14" s="49" t="s">
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
+      <c r="G14" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="51"/>
-      <c r="L14" s="49" t="s">
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="57"/>
+      <c r="L14" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="51"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="57"/>
       <c r="V14" s="21"/>
       <c r="W14" s="21"/>
       <c r="X14" s="21"/>
@@ -2079,36 +2064,36 @@
       <c r="Y18" s="21"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51"/>
-      <c r="G20" s="49" t="s">
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
+      <c r="G20" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="51"/>
-      <c r="L20" s="49" t="s">
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="57"/>
+      <c r="L20" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="51"/>
-      <c r="Q20" s="49" t="s">
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="57"/>
+      <c r="Q20" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="R20" s="50"/>
-      <c r="S20" s="50"/>
-      <c r="T20" s="51"/>
-      <c r="V20" s="49" t="s">
+      <c r="R20" s="56"/>
+      <c r="S20" s="56"/>
+      <c r="T20" s="57"/>
+      <c r="V20" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="W20" s="50"/>
-      <c r="X20" s="50"/>
-      <c r="Y20" s="51"/>
+      <c r="W20" s="56"/>
+      <c r="X20" s="56"/>
+      <c r="Y20" s="57"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
@@ -2351,36 +2336,36 @@
       </c>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="51"/>
-      <c r="G26" s="49" t="s">
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="57"/>
+      <c r="G26" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="51"/>
-      <c r="L26" s="49" t="s">
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="57"/>
+      <c r="L26" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="M26" s="50"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="51"/>
-      <c r="Q26" s="49" t="s">
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="57"/>
+      <c r="Q26" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="R26" s="50"/>
-      <c r="S26" s="50"/>
-      <c r="T26" s="51"/>
-      <c r="V26" s="49" t="s">
+      <c r="R26" s="56"/>
+      <c r="S26" s="56"/>
+      <c r="T26" s="57"/>
+      <c r="V26" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="W26" s="50"/>
-      <c r="X26" s="50"/>
-      <c r="Y26" s="51"/>
+      <c r="W26" s="56"/>
+      <c r="X26" s="56"/>
+      <c r="Y26" s="57"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B27" s="18"/>
@@ -2623,38 +2608,38 @@
       </c>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="51"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="57"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="49" t="s">
+      <c r="G32" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="51"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="57"/>
       <c r="K32" s="8"/>
-      <c r="L32" s="49" t="s">
+      <c r="L32" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="M32" s="50"/>
-      <c r="N32" s="50"/>
-      <c r="O32" s="51"/>
-      <c r="Q32" s="49" t="s">
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="57"/>
+      <c r="Q32" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="R32" s="50"/>
-      <c r="S32" s="50"/>
-      <c r="T32" s="51"/>
-      <c r="V32" s="49" t="s">
+      <c r="R32" s="56"/>
+      <c r="S32" s="56"/>
+      <c r="T32" s="57"/>
+      <c r="V32" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="W32" s="50"/>
-      <c r="X32" s="50"/>
-      <c r="Y32" s="51"/>
+      <c r="W32" s="56"/>
+      <c r="X32" s="56"/>
+      <c r="Y32" s="57"/>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B33" s="18" t="s">
@@ -2914,20 +2899,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="V20:Y20"/>
-    <mergeCell ref="V26:Y26"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="AH8:AI8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="V32:Y32"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="G14:J14"/>
@@ -2944,6 +2915,20 @@
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="L32:O32"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="AH8:AI8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="V20:Y20"/>
+    <mergeCell ref="V26:Y26"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="L8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2965,10 +2950,10 @@
       <c r="A1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="53"/>
+      <c r="F1" s="59"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
@@ -3039,7 +3024,7 @@
       <c r="A9" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="58" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3047,7 +3032,7 @@
       <c r="A10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="52"/>
+      <c r="B10" s="58"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
@@ -3150,10 +3135,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q33"/>
+  <dimension ref="B1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3165,490 +3150,753 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="73"/>
-      <c r="G2" s="71" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
-      <c r="N2" s="58" t="s">
+      <c r="B2" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="89"/>
+      <c r="G2" s="87" t="s">
         <v>79</v>
       </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="60"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="89"/>
+      <c r="N2" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="86"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="42" t="s">
+      <c r="B3" s="90"/>
+      <c r="C3" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="90" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="42" t="s">
+      <c r="E3" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="90"/>
+      <c r="H3" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="O3" s="62"/>
-      <c r="P3" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="64"/>
+      <c r="J3" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="61"/>
+      <c r="P3" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="73"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="87" t="s">
+      <c r="B4" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" s="65" t="s">
+      <c r="J4" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="66"/>
-      <c r="P4" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="68"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="75"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="31" t="s">
+      <c r="C5" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="N5" s="54" t="s">
-        <v>5</v>
-      </c>
-      <c r="O5" s="55"/>
-      <c r="P5" s="69" t="s">
+      <c r="J5" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="69"/>
+      <c r="P5" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="70"/>
+      <c r="Q5" s="77"/>
     </row>
     <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="26" t="s">
+      <c r="B6" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="25" t="s">
+      <c r="E6" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="24" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="73"/>
-      <c r="N9" s="58" t="s">
-        <v>77</v>
-      </c>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="60"/>
+      <c r="B9" s="87" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="89"/>
+      <c r="G9" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="89"/>
+      <c r="N9" s="84" t="s">
+        <v>80</v>
+      </c>
+      <c r="O9" s="85"/>
+      <c r="P9" s="85"/>
+      <c r="Q9" s="86"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="42" t="s">
+      <c r="B10" s="91"/>
+      <c r="C10" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="N10" s="61" t="s">
-        <v>4</v>
-      </c>
-      <c r="O10" s="62"/>
-      <c r="P10" s="74" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="75"/>
+      <c r="E10" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="90"/>
+      <c r="H10" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="O10" s="61"/>
+      <c r="P10" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="63"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="N11" s="65" t="s">
+      <c r="B11" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="66"/>
-      <c r="P11" s="76" t="s">
+      <c r="J11" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="Q11" s="77"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="67"/>
     </row>
     <row r="12" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="N12" s="54" t="s">
-        <v>5</v>
-      </c>
-      <c r="O12" s="55"/>
-      <c r="P12" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q12" s="57"/>
+      <c r="C12" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" s="69"/>
+      <c r="P12" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="71"/>
     </row>
     <row r="13" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>5</v>
+      <c r="B13" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="45" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="81"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="82"/>
-      <c r="C15" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="79" t="s">
+      <c r="B15" s="87" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="89"/>
+      <c r="G15" s="87" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="89"/>
+      <c r="N15" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="O15" s="85"/>
+      <c r="P15" s="85"/>
+      <c r="Q15" s="86"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="90"/>
+      <c r="C16" s="40">
+        <v>0</v>
+      </c>
+      <c r="D16" s="39">
+        <v>1</v>
+      </c>
+      <c r="E16" s="38">
+        <v>2</v>
+      </c>
+      <c r="G16" s="90"/>
+      <c r="H16" s="40">
+        <v>0</v>
+      </c>
+      <c r="I16" s="39">
+        <v>1</v>
+      </c>
+      <c r="J16" s="38">
+        <v>2</v>
+      </c>
+      <c r="N16" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="O16" s="61"/>
+      <c r="P16" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="80" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="33" t="s">
+      <c r="Q16" s="79"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="36">
+        <v>0</v>
+      </c>
+      <c r="C17" s="46">
+        <v>0</v>
+      </c>
+      <c r="D17" s="52">
+        <v>1</v>
+      </c>
+      <c r="E17" s="49">
+        <v>2</v>
+      </c>
+      <c r="G17" s="36">
+        <v>0</v>
+      </c>
+      <c r="H17" s="46">
+        <v>0</v>
+      </c>
+      <c r="I17" s="34">
+        <v>0</v>
+      </c>
+      <c r="J17" s="47">
+        <v>0</v>
+      </c>
+      <c r="N17" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="45"/>
-      <c r="C20" s="84" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="85" t="s">
+      <c r="O17" s="65"/>
+      <c r="P17" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="81"/>
+    </row>
+    <row r="18" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="31">
+        <v>1</v>
+      </c>
+      <c r="C18" s="50">
+        <v>1</v>
+      </c>
+      <c r="D18" s="93">
+        <v>2</v>
+      </c>
+      <c r="E18" s="43">
+        <v>0</v>
+      </c>
+      <c r="G18" s="31">
+        <v>1</v>
+      </c>
+      <c r="H18" s="30">
+        <v>0</v>
+      </c>
+      <c r="I18" s="41">
+        <v>0</v>
+      </c>
+      <c r="J18" s="51">
+        <v>1</v>
+      </c>
+      <c r="N18" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="69"/>
+      <c r="P18" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="83"/>
+    </row>
+    <row r="19" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="27">
+        <v>2</v>
+      </c>
+      <c r="C19" s="54">
+        <v>2</v>
+      </c>
+      <c r="D19" s="42">
+        <v>0</v>
+      </c>
+      <c r="E19" s="48">
+        <v>1</v>
+      </c>
+      <c r="G19" s="27">
+        <v>2</v>
+      </c>
+      <c r="H19" s="44">
+        <v>0</v>
+      </c>
+      <c r="I19" s="25">
+        <v>1</v>
+      </c>
+      <c r="J19" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="94"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="94"/>
+      <c r="N20" s="84" t="s">
+        <v>83</v>
+      </c>
+      <c r="O20" s="85"/>
+      <c r="P20" s="85"/>
+      <c r="Q20" s="86"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="94"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="94"/>
+      <c r="N21" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="61"/>
+      <c r="P21" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="63"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="94"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="N22" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="86" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="33" t="s">
+      <c r="O22" s="65"/>
+      <c r="P22" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="81"/>
+    </row>
+    <row r="23" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="94"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="N23" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="O23" s="69"/>
+      <c r="P23" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="71"/>
+    </row>
+    <row r="24" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="94"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
+      <c r="N25" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="O25" s="85"/>
+      <c r="P25" s="85"/>
+      <c r="Q25" s="86"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B26" s="94"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
+      <c r="E26" s="94"/>
+      <c r="N26" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="O26" s="61"/>
+      <c r="P26" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="73"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="94"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
+      <c r="N27" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="45"/>
-      <c r="C25" s="84" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="85" t="s">
+      <c r="O27" s="65"/>
+      <c r="P27" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q27" s="75"/>
+    </row>
+    <row r="28" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="94"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="N28" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="O28" s="69"/>
+      <c r="P28" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="71"/>
+    </row>
+    <row r="29" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B30" s="94"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="94"/>
+      <c r="N30" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="O30" s="85"/>
+      <c r="P30" s="85"/>
+      <c r="Q30" s="86"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B31" s="94"/>
+      <c r="C31" s="94"/>
+      <c r="D31" s="94"/>
+      <c r="E31" s="94"/>
+      <c r="N31" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="O31" s="61"/>
+      <c r="P31" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q31" s="73"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B32" s="94"/>
+      <c r="C32" s="94"/>
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="N32" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="86" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="33" t="s">
+      <c r="O32" s="65"/>
+      <c r="P32" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="81"/>
+    </row>
+    <row r="33" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="94"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="N33" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="O33" s="69"/>
+      <c r="P33" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q33" s="83"/>
+    </row>
+    <row r="34" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N35" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="O35" s="85"/>
+      <c r="P35" s="85"/>
+      <c r="Q35" s="86"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N36" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="O36" s="61"/>
+      <c r="P36" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="63"/>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N37" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="29" t="s">
+      <c r="O37" s="65"/>
+      <c r="P37" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="81"/>
+    </row>
+    <row r="38" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N38" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="O38" s="69"/>
+      <c r="P38" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="45"/>
-      <c r="C30" s="84" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="85" t="s">
+      <c r="Q38" s="77"/>
+    </row>
+    <row r="39" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N40" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="O40" s="85"/>
+      <c r="P40" s="85"/>
+      <c r="Q40" s="86"/>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N41" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="O41" s="61"/>
+      <c r="P41" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="86" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="33" t="s">
+      <c r="Q41" s="79"/>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="N42" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>4</v>
-      </c>
+      <c r="O42" s="65"/>
+      <c r="P42" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="75"/>
+    </row>
+    <row r="43" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N43" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="O43" s="69"/>
+      <c r="P43" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q43" s="71"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="62">
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="N40:Q40"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="G9:J9"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="N9:Q9"/>
     <mergeCell ref="N10:O10"/>
     <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
@@ -3658,6 +3906,6 @@
     <mergeCell ref="P5:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>